<commit_message>
Update of reference numbers
</commit_message>
<xml_diff>
--- a/data/FIT_RefIDsRefNo.xlsx
+++ b/data/FIT_RefIDsRefNo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirstenverostick/Documents/GitHub/ForensicIsoTissues/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E79057-7A33-EF4E-8A98-23468ABC2D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6842C381-2996-4440-8E86-612CBF35AA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="500" windowWidth="27640" windowHeight="16100" xr2:uid="{678B5CD5-4459-C646-AC2A-46C31D5BA5C9}"/>
+    <workbookView xWindow="320" yWindow="800" windowWidth="11040" windowHeight="16360" xr2:uid="{678B5CD5-4459-C646-AC2A-46C31D5BA5C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,24 +62,9 @@
     <t>Chesson et al. (2019)</t>
   </si>
   <si>
-    <t>Chesson et al. [36]</t>
-  </si>
-  <si>
-    <t>Gordon et al. [41]</t>
-  </si>
-  <si>
-    <t>Herrmann et al. [43]</t>
-  </si>
-  <si>
     <t>Regan [18]</t>
   </si>
   <si>
-    <t>Ueda &amp; Bell [27]</t>
-  </si>
-  <si>
-    <t>Kramer [42]</t>
-  </si>
-  <si>
     <t>Reference.ID</t>
   </si>
   <si>
@@ -92,16 +77,31 @@
     <t>Herrmann et al. (2015)</t>
   </si>
   <si>
-    <t>Engel [72]</t>
-  </si>
-  <si>
-    <t>Juarez [73]</t>
-  </si>
-  <si>
-    <t>Lustig [74]</t>
-  </si>
-  <si>
-    <t>Holobinko [96]</t>
+    <t>Engel [76]</t>
+  </si>
+  <si>
+    <t>Gordon et al. [45]</t>
+  </si>
+  <si>
+    <t>Herrmann et al. [47]</t>
+  </si>
+  <si>
+    <t>Juarez [78]</t>
+  </si>
+  <si>
+    <t>Lustig [79]</t>
+  </si>
+  <si>
+    <t>Kramer [46]</t>
+  </si>
+  <si>
+    <t>Holobinko [77]</t>
+  </si>
+  <si>
+    <t>Ueda &amp; Bell [29]</t>
+  </si>
+  <si>
+    <t>Chesson et al. [40]</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,10 +495,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -506,7 +506,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -514,23 +514,23 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -538,7 +538,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -554,7 +554,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -562,7 +562,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -570,7 +570,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -578,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last updates for figures with references
</commit_message>
<xml_diff>
--- a/data/FIT_RefIDsRefNo.xlsx
+++ b/data/FIT_RefIDsRefNo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirstenverostick/Documents/GitHub/ForensicIsoTissues/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6842C381-2996-4440-8E86-612CBF35AA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D78405-4C60-FD4D-BE19-B481978A6A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="800" windowWidth="11040" windowHeight="16360" xr2:uid="{678B5CD5-4459-C646-AC2A-46C31D5BA5C9}"/>
   </bookViews>
@@ -77,31 +77,31 @@
     <t>Herrmann et al. (2015)</t>
   </si>
   <si>
-    <t>Engel [76]</t>
-  </si>
-  <si>
     <t>Gordon et al. [45]</t>
   </si>
   <si>
     <t>Herrmann et al. [47]</t>
   </si>
   <si>
-    <t>Juarez [78]</t>
-  </si>
-  <si>
-    <t>Lustig [79]</t>
-  </si>
-  <si>
     <t>Kramer [46]</t>
   </si>
   <si>
-    <t>Holobinko [77]</t>
-  </si>
-  <si>
     <t>Ueda &amp; Bell [29]</t>
   </si>
   <si>
     <t>Chesson et al. [40]</t>
+  </si>
+  <si>
+    <t>Holobinko [75]</t>
+  </si>
+  <si>
+    <t>Juarez [76]</t>
+  </si>
+  <si>
+    <t>Lustig [77]</t>
+  </si>
+  <si>
+    <t>Engel [74]</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,7 +506,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -514,7 +514,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -522,7 +522,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -530,7 +530,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -538,7 +538,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -554,7 +554,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -570,7 +570,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -578,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>